<commit_message>
nova bible math book
</commit_message>
<xml_diff>
--- a/GRE/Roadmap/Practice.xlsx
+++ b/GRE/Roadmap/Practice.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9000" windowWidth="22260" windowHeight="12645" tabRatio="556" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="9450" windowWidth="22260" windowHeight="12645" tabRatio="556" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Catalogue" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="245">
   <si>
     <t>Number</t>
   </si>
@@ -697,13 +697,73 @@
   </si>
   <si>
     <t>integer constraint,</t>
+  </si>
+  <si>
+    <t>B E H</t>
+  </si>
+  <si>
+    <t>4_Divisibility and Primes</t>
+  </si>
+  <si>
+    <t>A C E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B </t>
+  </si>
+  <si>
+    <t>D E</t>
+  </si>
+  <si>
+    <t>12!</t>
+  </si>
+  <si>
+    <t>A E F</t>
+  </si>
+  <si>
+    <t>A B C D</t>
+  </si>
+  <si>
+    <t>14|Exponents and Roots</t>
+  </si>
+  <si>
+    <t>test_14</t>
+  </si>
+  <si>
+    <t>1_2</t>
+  </si>
+  <si>
+    <t>2^96</t>
+  </si>
+  <si>
+    <t>5_Word Problems</t>
+  </si>
+  <si>
+    <t>60s</t>
+  </si>
+  <si>
+    <t>48h</t>
+  </si>
+  <si>
+    <t>9y</t>
+  </si>
+  <si>
+    <t>2.57m</t>
+  </si>
+  <si>
+    <t>1x10^7</t>
+  </si>
+  <si>
+    <t>20/49</t>
+  </si>
+  <si>
+    <t>38_75</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -715,6 +775,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -761,10 +836,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -799,6 +875,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -807,11 +886,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1090,10 +1170,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="J8" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,7 +1292,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G19" si="0">D4/(D4+E4+F4)*100</f>
+        <f t="shared" ref="G4:G20" si="0">D4/(D4+E4+F4)*100</f>
         <v>75</v>
       </c>
       <c r="H4" t="s">
@@ -1592,19 +1672,19 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="23" t="s">
         <v>223</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -1637,6 +1717,36 @@
       </c>
       <c r="K19" t="s">
         <v>224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <v>32</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>82.051282051282044</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="I20" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -1670,7 +1780,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G13:G17 G19">
+  <conditionalFormatting sqref="G13:G17 G19:G20">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="70"/>
@@ -1699,10 +1809,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S74"/>
+  <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1714,11 +1824,11 @@
     <col min="18" max="18" width="3.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1733,7 +1843,7 @@
       <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="24" t="s">
         <v>122</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1748,7 +1858,7 @@
       <c r="K1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="24" t="s">
         <v>121</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -1766,18 +1876,21 @@
       <c r="Q1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="R1" s="24" t="s">
         <v>222</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
+      <c r="B2" s="24"/>
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1790,7 +1903,7 @@
       <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="23"/>
+      <c r="G2" s="24"/>
       <c r="H2" t="s">
         <v>13</v>
       </c>
@@ -1803,7 +1916,7 @@
       <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="23"/>
+      <c r="L2" s="24"/>
       <c r="M2" t="s">
         <v>125</v>
       </c>
@@ -1819,16 +1932,19 @@
       <c r="Q2" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="23"/>
+      <c r="R2" s="24"/>
       <c r="S2" s="3">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1841,7 +1957,7 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="23"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="4"/>
       <c r="I3">
         <v>1</v>
@@ -1852,7 +1968,7 @@
       <c r="K3" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="23"/>
+      <c r="L3" s="24"/>
       <c r="M3" t="s">
         <v>13</v>
       </c>
@@ -1868,16 +1984,19 @@
       <c r="Q3">
         <v>80</v>
       </c>
-      <c r="R3" s="23"/>
+      <c r="R3" s="24"/>
       <c r="S3" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="23"/>
+      <c r="B4" s="24"/>
       <c r="C4" t="s">
         <v>11</v>
       </c>
@@ -1890,7 +2009,7 @@
       <c r="F4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="23"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="3">
         <v>118</v>
       </c>
@@ -1903,7 +2022,7 @@
       <c r="K4" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="23"/>
+      <c r="L4" s="24"/>
       <c r="M4" t="s">
         <v>13</v>
       </c>
@@ -1919,16 +2038,19 @@
       <c r="Q4" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="23"/>
+      <c r="R4" s="24"/>
       <c r="S4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="23"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1941,7 +2063,7 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="23"/>
+      <c r="G5" s="24"/>
       <c r="H5" s="3">
         <v>12</v>
       </c>
@@ -1955,7 +2077,7 @@
       <c r="K5">
         <v>37</v>
       </c>
-      <c r="L5" s="23"/>
+      <c r="L5" s="24"/>
       <c r="M5" s="4"/>
       <c r="N5" t="s">
         <v>11</v>
@@ -1969,16 +2091,19 @@
       <c r="Q5">
         <v>20</v>
       </c>
-      <c r="R5" s="23"/>
+      <c r="R5" s="24"/>
       <c r="S5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="23"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1991,7 +2116,7 @@
       <c r="F6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="23"/>
+      <c r="G6" s="24"/>
       <c r="H6" s="5" t="s">
         <v>10</v>
       </c>
@@ -2004,7 +2129,7 @@
       <c r="K6">
         <v>720</v>
       </c>
-      <c r="L6" s="23"/>
+      <c r="L6" s="24"/>
       <c r="M6" s="4"/>
       <c r="N6" t="s">
         <v>11</v>
@@ -2018,16 +2143,19 @@
       <c r="Q6" t="s">
         <v>12</v>
       </c>
-      <c r="R6" s="23"/>
+      <c r="R6" s="24"/>
       <c r="S6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="24"/>
       <c r="C7" t="s">
         <v>10</v>
       </c>
@@ -2040,7 +2168,7 @@
       <c r="F7" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="23"/>
+      <c r="G7" s="24"/>
       <c r="H7">
         <v>7.5</v>
       </c>
@@ -2053,7 +2181,7 @@
       <c r="K7" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="23"/>
+      <c r="L7" s="24"/>
       <c r="M7" s="19" t="s">
         <v>126</v>
       </c>
@@ -2069,16 +2197,19 @@
       <c r="Q7">
         <v>30</v>
       </c>
-      <c r="R7" s="23"/>
+      <c r="R7" s="24"/>
       <c r="S7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="23"/>
+      <c r="B8" s="24"/>
       <c r="C8" t="s">
         <v>11</v>
       </c>
@@ -2091,7 +2222,7 @@
       <c r="F8" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="23"/>
+      <c r="G8" s="24"/>
       <c r="H8" t="s">
         <v>10</v>
       </c>
@@ -2104,7 +2235,7 @@
       <c r="K8">
         <v>2</v>
       </c>
-      <c r="L8" s="23"/>
+      <c r="L8" s="24"/>
       <c r="M8" t="s">
         <v>127</v>
       </c>
@@ -2120,16 +2251,19 @@
       <c r="Q8">
         <v>11</v>
       </c>
-      <c r="R8" s="23"/>
+      <c r="R8" s="24"/>
       <c r="S8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="23"/>
+      <c r="B9" s="24"/>
       <c r="C9" t="s">
         <v>10</v>
       </c>
@@ -2142,7 +2276,7 @@
       <c r="F9" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="23"/>
+      <c r="G9" s="24"/>
       <c r="H9" t="s">
         <v>12</v>
       </c>
@@ -2155,7 +2289,7 @@
       <c r="K9">
         <v>1</v>
       </c>
-      <c r="L9" s="23"/>
+      <c r="L9" s="24"/>
       <c r="M9" s="3" t="s">
         <v>128</v>
       </c>
@@ -2171,16 +2305,19 @@
       <c r="Q9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="R9" s="23"/>
+      <c r="R9" s="24"/>
       <c r="S9" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="23"/>
+      <c r="B10" s="24"/>
       <c r="C10" t="s">
         <v>10</v>
       </c>
@@ -2193,7 +2330,7 @@
       <c r="F10" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="23"/>
+      <c r="G10" s="24"/>
       <c r="H10" t="s">
         <v>12</v>
       </c>
@@ -2206,7 +2343,7 @@
       <c r="K10" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="23"/>
+      <c r="L10" s="24"/>
       <c r="M10" t="s">
         <v>13</v>
       </c>
@@ -2222,16 +2359,19 @@
       <c r="Q10" s="5">
         <v>10</v>
       </c>
-      <c r="R10" s="23"/>
+      <c r="R10" s="24"/>
       <c r="S10" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="23"/>
+      <c r="B11" s="24"/>
       <c r="C11">
         <v>7.4</v>
       </c>
@@ -2244,7 +2384,7 @@
       <c r="F11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="23"/>
+      <c r="G11" s="24"/>
       <c r="H11">
         <v>144</v>
       </c>
@@ -2257,7 +2397,7 @@
       <c r="K11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L11" s="23"/>
+      <c r="L11" s="24"/>
       <c r="M11" t="s">
         <v>11</v>
       </c>
@@ -2273,16 +2413,19 @@
       <c r="Q11" t="s">
         <v>12</v>
       </c>
-      <c r="R11" s="23"/>
+      <c r="R11" s="24"/>
       <c r="S11" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="23"/>
+      <c r="B12" s="24"/>
       <c r="C12" t="s">
         <v>10</v>
       </c>
@@ -2295,7 +2438,7 @@
       <c r="F12">
         <v>216</v>
       </c>
-      <c r="G12" s="23"/>
+      <c r="G12" s="24"/>
       <c r="H12" t="s">
         <v>21</v>
       </c>
@@ -2306,7 +2449,7 @@
         <v>50</v>
       </c>
       <c r="K12" s="4"/>
-      <c r="L12" s="23"/>
+      <c r="L12" s="24"/>
       <c r="M12" t="s">
         <v>13</v>
       </c>
@@ -2322,16 +2465,19 @@
       <c r="Q12" t="s">
         <v>10</v>
       </c>
-      <c r="R12" s="23"/>
+      <c r="R12" s="24"/>
       <c r="S12" s="5" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T12" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="23"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3">
         <v>143</v>
@@ -2340,7 +2486,7 @@
         <v>10</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="23"/>
+      <c r="G13" s="24"/>
       <c r="H13" t="s">
         <v>11</v>
       </c>
@@ -2353,7 +2499,7 @@
       <c r="K13" s="3">
         <v>19.312000000000001</v>
       </c>
-      <c r="L13" s="23"/>
+      <c r="L13" s="24"/>
       <c r="M13" t="s">
         <v>11</v>
       </c>
@@ -2369,16 +2515,19 @@
       <c r="Q13">
         <v>12</v>
       </c>
-      <c r="R13" s="23"/>
+      <c r="R13" s="24"/>
       <c r="S13">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T13" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="23"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="3">
         <v>2</v>
       </c>
@@ -2391,7 +2540,7 @@
       <c r="F14" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="23"/>
+      <c r="G14" s="24"/>
       <c r="H14" t="s">
         <v>12</v>
       </c>
@@ -2404,7 +2553,7 @@
       <c r="K14">
         <v>43</v>
       </c>
-      <c r="L14" s="23"/>
+      <c r="L14" s="24"/>
       <c r="M14" s="3" t="s">
         <v>129</v>
       </c>
@@ -2418,16 +2567,19 @@
         <v>11</v>
       </c>
       <c r="Q14" s="4"/>
-      <c r="R14" s="23"/>
+      <c r="R14" s="24"/>
       <c r="S14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T14" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="23"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="3" t="s">
         <v>14</v>
       </c>
@@ -2440,7 +2592,7 @@
       <c r="F15" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="23"/>
+      <c r="G15" s="24"/>
       <c r="H15" s="3" t="s">
         <v>12</v>
       </c>
@@ -2453,7 +2605,7 @@
       <c r="K15">
         <v>15</v>
       </c>
-      <c r="L15" s="23"/>
+      <c r="L15" s="24"/>
       <c r="M15" s="3" t="s">
         <v>11</v>
       </c>
@@ -2469,22 +2621,25 @@
       <c r="Q15" t="s">
         <v>11</v>
       </c>
-      <c r="R15" s="23"/>
+      <c r="R15" s="24"/>
       <c r="S15" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T15" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="23"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="4"/>
       <c r="D16" t="s">
         <v>12</v>
       </c>
       <c r="F16"/>
-      <c r="G16" s="23"/>
+      <c r="G16" s="24"/>
       <c r="H16" t="s">
         <v>10</v>
       </c>
@@ -2497,7 +2652,7 @@
       <c r="K16" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="L16" s="23"/>
+      <c r="L16" s="24"/>
       <c r="M16" t="s">
         <v>130</v>
       </c>
@@ -2513,16 +2668,19 @@
       <c r="Q16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R16" s="23"/>
+      <c r="R16" s="24"/>
       <c r="S16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T16" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="23"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
@@ -2530,7 +2688,7 @@
         <v>11</v>
       </c>
       <c r="F17"/>
-      <c r="G17" s="23"/>
+      <c r="G17" s="24"/>
       <c r="H17" t="s">
         <v>11</v>
       </c>
@@ -2543,7 +2701,7 @@
       <c r="K17" t="s">
         <v>67</v>
       </c>
-      <c r="L17" s="23"/>
+      <c r="L17" s="24"/>
       <c r="M17" t="s">
         <v>12</v>
       </c>
@@ -2559,14 +2717,15 @@
       <c r="Q17" t="s">
         <v>13</v>
       </c>
-      <c r="R17" s="23"/>
+      <c r="R17" s="24"/>
       <c r="S17" s="4"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T17" s="4"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="23"/>
+      <c r="B18" s="24"/>
       <c r="C18" t="s">
         <v>11</v>
       </c>
@@ -2574,7 +2733,7 @@
         <v>9</v>
       </c>
       <c r="F18"/>
-      <c r="G18" s="23"/>
+      <c r="G18" s="24"/>
       <c r="H18" t="s">
         <v>11</v>
       </c>
@@ -2587,7 +2746,7 @@
       <c r="K18">
         <v>0</v>
       </c>
-      <c r="L18" s="23"/>
+      <c r="L18" s="24"/>
       <c r="M18" s="3" t="s">
         <v>13</v>
       </c>
@@ -2603,16 +2762,19 @@
       <c r="Q18" t="s">
         <v>12</v>
       </c>
-      <c r="R18" s="23"/>
+      <c r="R18" s="24"/>
       <c r="S18" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T18" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="24"/>
       <c r="C19" t="s">
         <v>11</v>
       </c>
@@ -2620,7 +2782,7 @@
         <v>11</v>
       </c>
       <c r="F19"/>
-      <c r="G19" s="23"/>
+      <c r="G19" s="24"/>
       <c r="H19" t="s">
         <v>12</v>
       </c>
@@ -2634,7 +2796,7 @@
       <c r="K19" t="s">
         <v>12</v>
       </c>
-      <c r="L19" s="23"/>
+      <c r="L19" s="24"/>
       <c r="M19" t="s">
         <v>12</v>
       </c>
@@ -2650,14 +2812,17 @@
       <c r="Q19" t="s">
         <v>11</v>
       </c>
-      <c r="R19" s="23"/>
+      <c r="R19" s="24"/>
       <c r="S19" s="4"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="23"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="3" t="s">
         <v>13</v>
       </c>
@@ -2665,7 +2830,7 @@
         <v>13</v>
       </c>
       <c r="F20"/>
-      <c r="G20" s="23"/>
+      <c r="G20" s="24"/>
       <c r="I20">
         <v>30</v>
       </c>
@@ -2675,7 +2840,7 @@
       <c r="K20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L20" s="23"/>
+      <c r="L20" s="24"/>
       <c r="M20" s="3" t="s">
         <v>10</v>
       </c>
@@ -2691,16 +2856,19 @@
       <c r="Q20" t="s">
         <v>10</v>
       </c>
-      <c r="R20" s="23"/>
+      <c r="R20" s="24"/>
       <c r="S20" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T20" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="23"/>
+      <c r="B21" s="24"/>
       <c r="C21" t="s">
         <v>11</v>
       </c>
@@ -2708,7 +2876,7 @@
         <v>13</v>
       </c>
       <c r="F21"/>
-      <c r="G21" s="23"/>
+      <c r="G21" s="24"/>
       <c r="I21">
         <v>9</v>
       </c>
@@ -2718,7 +2886,7 @@
       <c r="K21" t="s">
         <v>13</v>
       </c>
-      <c r="L21" s="23"/>
+      <c r="L21" s="24"/>
       <c r="M21" s="3" t="s">
         <v>131</v>
       </c>
@@ -2734,21 +2902,24 @@
       <c r="Q21" t="s">
         <v>13</v>
       </c>
-      <c r="R21" s="23"/>
+      <c r="R21" s="24"/>
       <c r="S21" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="23"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
-      <c r="G22" s="23"/>
+      <c r="G22" s="24"/>
       <c r="I22">
         <v>3</v>
       </c>
@@ -2758,7 +2929,7 @@
       <c r="K22" t="s">
         <v>11</v>
       </c>
-      <c r="L22" s="23"/>
+      <c r="L22" s="24"/>
       <c r="M22" t="s">
         <v>11</v>
       </c>
@@ -2774,21 +2945,24 @@
       <c r="Q22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R22" s="23"/>
+      <c r="R22" s="24"/>
       <c r="S22" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T22">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="23"/>
+      <c r="B23" s="24"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
-      <c r="G23" s="23"/>
+      <c r="G23" s="24"/>
       <c r="I23">
         <v>1</v>
       </c>
@@ -2798,7 +2972,7 @@
       <c r="K23" s="3">
         <v>270</v>
       </c>
-      <c r="L23" s="23"/>
+      <c r="L23" s="24"/>
       <c r="M23" t="s">
         <v>11</v>
       </c>
@@ -2814,21 +2988,24 @@
       <c r="Q23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="R23" s="23"/>
+      <c r="R23" s="24"/>
       <c r="S23" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T23">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="23"/>
+      <c r="B24" s="24"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
-      <c r="G24" s="23"/>
+      <c r="G24" s="24"/>
       <c r="I24" s="3">
         <v>12</v>
       </c>
@@ -2838,7 +3015,7 @@
       <c r="K24" t="s">
         <v>21</v>
       </c>
-      <c r="L24" s="23"/>
+      <c r="L24" s="24"/>
       <c r="M24" t="s">
         <v>12</v>
       </c>
@@ -2854,21 +3031,24 @@
       <c r="Q24" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="R24" s="23"/>
+      <c r="R24" s="24"/>
       <c r="S24" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T24" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="23"/>
+      <c r="B25" s="24"/>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
-      <c r="G25" s="23"/>
+      <c r="G25" s="24"/>
       <c r="I25" t="s">
         <v>12</v>
       </c>
@@ -2878,7 +3058,7 @@
       <c r="K25" t="s">
         <v>10</v>
       </c>
-      <c r="L25" s="23"/>
+      <c r="L25" s="24"/>
       <c r="M25" s="3" t="s">
         <v>10</v>
       </c>
@@ -2894,19 +3074,22 @@
       <c r="Q25" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="R25" s="23"/>
+      <c r="R25" s="24"/>
       <c r="S25" s="4"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T25" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="23"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
-      <c r="G26" s="23"/>
+      <c r="G26" s="24"/>
       <c r="I26" t="s">
         <v>13</v>
       </c>
@@ -2916,7 +3099,7 @@
       <c r="K26" t="s">
         <v>13</v>
       </c>
-      <c r="L26" s="23"/>
+      <c r="L26" s="24"/>
       <c r="M26" t="s">
         <v>13</v>
       </c>
@@ -2932,21 +3115,24 @@
       <c r="Q26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R26" s="23"/>
+      <c r="R26" s="24"/>
       <c r="S26" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T26" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="23"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
-      <c r="G27" s="23"/>
+      <c r="G27" s="24"/>
       <c r="I27" s="8" t="s">
         <v>10</v>
       </c>
@@ -2954,7 +3140,7 @@
         <v>11</v>
       </c>
       <c r="K27" s="4"/>
-      <c r="L27" s="23"/>
+      <c r="L27" s="24"/>
       <c r="M27" t="s">
         <v>21</v>
       </c>
@@ -2970,19 +3156,20 @@
       <c r="Q27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="R27" s="23"/>
+      <c r="R27" s="24"/>
       <c r="S27" s="4"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T27" s="4"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="23"/>
+      <c r="B28" s="24"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
-      <c r="G28" s="23"/>
+      <c r="G28" s="24"/>
       <c r="I28" s="8" t="s">
         <v>11</v>
       </c>
@@ -2990,7 +3177,7 @@
         <v>10</v>
       </c>
       <c r="K28" s="4"/>
-      <c r="L28" s="23"/>
+      <c r="L28" s="24"/>
       <c r="M28" s="15" t="s">
         <v>132</v>
       </c>
@@ -3004,21 +3191,24 @@
       <c r="Q28" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="R28" s="23"/>
+      <c r="R28" s="24"/>
       <c r="S28" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="23"/>
+      <c r="B29" s="24"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
-      <c r="G29" s="23"/>
+      <c r="G29" s="24"/>
       <c r="I29" s="8" t="s">
         <v>11</v>
       </c>
@@ -3028,7 +3218,7 @@
       <c r="K29">
         <v>1778</v>
       </c>
-      <c r="L29" s="23"/>
+      <c r="L29" s="24"/>
       <c r="M29" s="4"/>
       <c r="N29" t="s">
         <v>142</v>
@@ -3042,21 +3232,24 @@
       <c r="Q29" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="R29" s="23"/>
+      <c r="R29" s="24"/>
       <c r="S29" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T29" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="23"/>
+      <c r="B30" s="24"/>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
-      <c r="G30" s="23"/>
+      <c r="G30" s="24"/>
       <c r="I30" s="8" t="s">
         <v>12</v>
       </c>
@@ -3066,7 +3259,7 @@
       <c r="K30" t="s">
         <v>13</v>
       </c>
-      <c r="L30" s="23"/>
+      <c r="L30" s="24"/>
       <c r="M30" s="5" t="s">
         <v>13</v>
       </c>
@@ -3082,21 +3275,24 @@
       <c r="Q30" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="R30" s="23"/>
+      <c r="R30" s="24"/>
       <c r="S30" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T30" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="23"/>
+      <c r="B31" s="24"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
-      <c r="G31" s="23"/>
+      <c r="G31" s="24"/>
       <c r="I31" s="9" t="s">
         <v>13</v>
       </c>
@@ -3106,7 +3302,7 @@
       <c r="K31" t="s">
         <v>10</v>
       </c>
-      <c r="L31" s="23"/>
+      <c r="L31" s="24"/>
       <c r="M31" s="5" t="s">
         <v>10</v>
       </c>
@@ -3122,21 +3318,24 @@
       <c r="Q31" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R31" s="23"/>
+      <c r="R31" s="24"/>
       <c r="S31" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T31" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="23"/>
+      <c r="B32" s="24"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
-      <c r="G32" s="23"/>
+      <c r="G32" s="24"/>
       <c r="I32" s="9" t="s">
         <v>13</v>
       </c>
@@ -3144,7 +3343,7 @@
       <c r="K32" t="s">
         <v>11</v>
       </c>
-      <c r="L32" s="23"/>
+      <c r="L32" s="24"/>
       <c r="M32" s="5" t="s">
         <v>11</v>
       </c>
@@ -3160,21 +3359,24 @@
       <c r="Q32" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="R32" s="23"/>
+      <c r="R32" s="24"/>
       <c r="S32" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T32" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="23"/>
+      <c r="B33" s="24"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
-      <c r="G33" s="23"/>
+      <c r="G33" s="24"/>
       <c r="I33" s="9" t="s">
         <v>13</v>
       </c>
@@ -3184,7 +3386,7 @@
       <c r="K33" t="s">
         <v>21</v>
       </c>
-      <c r="L33" s="23"/>
+      <c r="L33" s="24"/>
       <c r="M33" s="3" t="s">
         <v>12</v>
       </c>
@@ -3195,21 +3397,24 @@
         <v>13</v>
       </c>
       <c r="Q33" s="4"/>
-      <c r="R33" s="23"/>
+      <c r="R33" s="24"/>
       <c r="S33" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T33" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="23"/>
+      <c r="B34" s="24"/>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
-      <c r="G34" s="23"/>
+      <c r="G34" s="24"/>
       <c r="I34" s="9" t="s">
         <v>19</v>
       </c>
@@ -3219,7 +3424,7 @@
       <c r="K34" t="s">
         <v>10</v>
       </c>
-      <c r="L34" s="23"/>
+      <c r="L34" s="24"/>
       <c r="M34" s="3" t="s">
         <v>21</v>
       </c>
@@ -3232,21 +3437,24 @@
       <c r="Q34" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="R34" s="23"/>
+      <c r="R34" s="24"/>
       <c r="S34" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T34" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="23"/>
+      <c r="B35" s="24"/>
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
-      <c r="G35" s="23"/>
+      <c r="G35" s="24"/>
       <c r="I35" s="8" t="s">
         <v>12</v>
       </c>
@@ -3256,7 +3464,7 @@
       <c r="K35" t="s">
         <v>13</v>
       </c>
-      <c r="L35" s="23"/>
+      <c r="L35" s="24"/>
       <c r="M35" s="3" t="s">
         <v>133</v>
       </c>
@@ -3269,21 +3477,24 @@
       <c r="Q35" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="R35" s="23"/>
+      <c r="R35" s="24"/>
       <c r="S35" s="3" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T35" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="23"/>
+      <c r="B36" s="24"/>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
-      <c r="G36" s="23"/>
+      <c r="G36" s="24"/>
       <c r="I36" s="8" t="s">
         <v>10</v>
       </c>
@@ -3293,7 +3504,7 @@
       <c r="K36" t="s">
         <v>10</v>
       </c>
-      <c r="L36" s="23"/>
+      <c r="L36" s="24"/>
       <c r="M36" s="3" t="s">
         <v>10</v>
       </c>
@@ -3303,21 +3514,24 @@
       <c r="Q36" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="R36" s="23"/>
+      <c r="R36" s="24"/>
       <c r="S36" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T36" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="23"/>
+      <c r="B37" s="24"/>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
       <c r="E37" s="13"/>
       <c r="F37" s="13"/>
-      <c r="G37" s="23"/>
+      <c r="G37" s="24"/>
       <c r="I37" s="8" t="s">
         <v>10</v>
       </c>
@@ -3327,7 +3541,7 @@
       <c r="K37" t="s">
         <v>12</v>
       </c>
-      <c r="L37" s="23"/>
+      <c r="L37" s="24"/>
       <c r="M37" s="3" t="s">
         <v>10</v>
       </c>
@@ -3337,19 +3551,22 @@
       <c r="Q37" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="R37" s="23"/>
+      <c r="R37" s="24"/>
       <c r="S37" s="4"/>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T37" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="23"/>
+      <c r="B38" s="24"/>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
-      <c r="G38" s="23"/>
+      <c r="G38" s="24"/>
       <c r="I38" s="9" t="s">
         <v>10</v>
       </c>
@@ -3359,7 +3576,7 @@
       <c r="K38" t="s">
         <v>21</v>
       </c>
-      <c r="L38" s="23"/>
+      <c r="L38" s="24"/>
       <c r="M38" s="5" t="s">
         <v>12</v>
       </c>
@@ -3369,21 +3586,24 @@
       <c r="Q38" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="R38" s="23"/>
+      <c r="R38" s="24"/>
       <c r="S38">
         <v>110</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T38" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="23"/>
+      <c r="B39" s="24"/>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
       <c r="E39" s="13"/>
       <c r="F39" s="13"/>
-      <c r="G39" s="23"/>
+      <c r="G39" s="24"/>
       <c r="I39" s="8" t="s">
         <v>12</v>
       </c>
@@ -3393,7 +3613,7 @@
       <c r="K39" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L39" s="23"/>
+      <c r="L39" s="24"/>
       <c r="M39" s="3" t="s">
         <v>11</v>
       </c>
@@ -3403,21 +3623,24 @@
       <c r="Q39" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R39" s="23"/>
+      <c r="R39" s="24"/>
       <c r="S39" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T39" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="23"/>
+      <c r="B40" s="24"/>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
       <c r="F40" s="13"/>
-      <c r="G40" s="23"/>
+      <c r="G40" s="24"/>
       <c r="I40" s="8" t="s">
         <v>10</v>
       </c>
@@ -3427,7 +3650,7 @@
       <c r="K40" t="s">
         <v>11</v>
       </c>
-      <c r="L40" s="23"/>
+      <c r="L40" s="24"/>
       <c r="M40" s="20" t="s">
         <v>128</v>
       </c>
@@ -3435,21 +3658,24 @@
         <v>144</v>
       </c>
       <c r="Q40" s="4"/>
-      <c r="R40" s="23"/>
+      <c r="R40" s="24"/>
       <c r="S40" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T40" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="23"/>
+      <c r="B41" s="24"/>
       <c r="C41" s="13"/>
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
       <c r="F41" s="13"/>
-      <c r="G41" s="23"/>
+      <c r="G41" s="24"/>
       <c r="I41" s="8" t="s">
         <v>12</v>
       </c>
@@ -3459,7 +3685,7 @@
       <c r="K41" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L41" s="23"/>
+      <c r="L41" s="24"/>
       <c r="M41" s="18" t="s">
         <v>134</v>
       </c>
@@ -3469,19 +3695,19 @@
       <c r="Q41" t="s">
         <v>12</v>
       </c>
-      <c r="R41" s="23"/>
+      <c r="R41" s="24"/>
       <c r="S41" s="4"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="23"/>
+      <c r="B42" s="24"/>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
       <c r="E42" s="13"/>
       <c r="F42" s="13"/>
-      <c r="G42" s="23"/>
+      <c r="G42" s="24"/>
       <c r="I42" s="9" t="s">
         <v>13</v>
       </c>
@@ -3491,7 +3717,7 @@
       <c r="K42" t="s">
         <v>10</v>
       </c>
-      <c r="L42" s="23"/>
+      <c r="L42" s="24"/>
       <c r="M42" s="18" t="s">
         <v>135</v>
       </c>
@@ -3501,19 +3727,19 @@
       <c r="Q42" t="s">
         <v>10</v>
       </c>
-      <c r="R42" s="23"/>
+      <c r="R42" s="24"/>
       <c r="S42" s="4"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="23"/>
+      <c r="B43" s="24"/>
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
       <c r="E43" s="13"/>
       <c r="F43" s="13"/>
-      <c r="G43" s="23"/>
+      <c r="G43" s="24"/>
       <c r="I43">
         <v>-3</v>
       </c>
@@ -3523,7 +3749,7 @@
       <c r="K43" t="s">
         <v>11</v>
       </c>
-      <c r="L43" s="23"/>
+      <c r="L43" s="24"/>
       <c r="M43" s="18" t="s">
         <v>10</v>
       </c>
@@ -3533,19 +3759,19 @@
       <c r="Q43" t="s">
         <v>12</v>
       </c>
-      <c r="R43" s="23"/>
+      <c r="R43" s="24"/>
       <c r="S43" s="4"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="23"/>
+      <c r="B44" s="24"/>
       <c r="C44" s="13"/>
       <c r="D44" s="13"/>
       <c r="E44" s="13"/>
       <c r="F44" s="13"/>
-      <c r="G44" s="23"/>
+      <c r="G44" s="24"/>
       <c r="I44">
         <v>6</v>
       </c>
@@ -3555,7 +3781,7 @@
       <c r="K44" t="s">
         <v>10</v>
       </c>
-      <c r="L44" s="23"/>
+      <c r="L44" s="24"/>
       <c r="M44" s="18" t="s">
         <v>11</v>
       </c>
@@ -3563,19 +3789,19 @@
         <v>11</v>
       </c>
       <c r="Q44" s="4"/>
-      <c r="R44" s="23"/>
+      <c r="R44" s="24"/>
       <c r="S44" s="4"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="23"/>
+      <c r="B45" s="24"/>
       <c r="C45" s="13"/>
       <c r="D45" s="13"/>
       <c r="E45" s="13"/>
       <c r="F45" s="13"/>
-      <c r="G45" s="23"/>
+      <c r="G45" s="24"/>
       <c r="I45">
         <v>4</v>
       </c>
@@ -3585,7 +3811,7 @@
       <c r="K45" t="s">
         <v>11</v>
       </c>
-      <c r="L45" s="23"/>
+      <c r="L45" s="24"/>
       <c r="M45" s="20" t="s">
         <v>13</v>
       </c>
@@ -3595,19 +3821,19 @@
       <c r="Q45" t="s">
         <v>12</v>
       </c>
-      <c r="R45" s="23"/>
+      <c r="R45" s="24"/>
       <c r="S45" s="4"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="23"/>
+      <c r="B46" s="24"/>
       <c r="C46" s="13"/>
       <c r="D46" s="13"/>
       <c r="E46" s="13"/>
       <c r="F46" s="13"/>
-      <c r="G46" s="23"/>
+      <c r="G46" s="24"/>
       <c r="I46" t="s">
         <v>10</v>
       </c>
@@ -3615,7 +3841,7 @@
       <c r="K46" t="s">
         <v>10</v>
       </c>
-      <c r="L46" s="23"/>
+      <c r="L46" s="24"/>
       <c r="M46" s="18" t="s">
         <v>13</v>
       </c>
@@ -3623,18 +3849,18 @@
         <v>13</v>
       </c>
       <c r="Q46" s="4"/>
-      <c r="R46" s="23"/>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R46" s="24"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="23"/>
+      <c r="B47" s="24"/>
       <c r="C47" s="13"/>
       <c r="D47" s="13"/>
       <c r="E47" s="13"/>
       <c r="F47" s="13"/>
-      <c r="G47" s="23"/>
+      <c r="G47" s="24"/>
       <c r="I47" s="5" t="s">
         <v>14</v>
       </c>
@@ -3644,7 +3870,7 @@
       <c r="K47" t="s">
         <v>11</v>
       </c>
-      <c r="L47" s="23"/>
+      <c r="L47" s="24"/>
       <c r="M47" s="18" t="s">
         <v>13</v>
       </c>
@@ -3654,18 +3880,18 @@
       <c r="Q47" t="s">
         <v>10</v>
       </c>
-      <c r="R47" s="23"/>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R47" s="24"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="23"/>
+      <c r="B48" s="24"/>
       <c r="C48" s="13"/>
       <c r="D48" s="13"/>
       <c r="E48" s="13"/>
       <c r="F48" s="13"/>
-      <c r="G48" s="23"/>
+      <c r="G48" s="24"/>
       <c r="I48" t="s">
         <v>10</v>
       </c>
@@ -3673,7 +3899,7 @@
         <v>13</v>
       </c>
       <c r="K48" s="4"/>
-      <c r="L48" s="23"/>
+      <c r="L48" s="24"/>
       <c r="M48" s="20" t="s">
         <v>10</v>
       </c>
@@ -3683,18 +3909,18 @@
       <c r="Q48" t="s">
         <v>10</v>
       </c>
-      <c r="R48" s="23"/>
+      <c r="R48" s="24"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="23"/>
+      <c r="B49" s="24"/>
       <c r="C49" s="13"/>
       <c r="D49" s="13"/>
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
-      <c r="G49" s="23"/>
+      <c r="G49" s="24"/>
       <c r="I49" t="s">
         <v>12</v>
       </c>
@@ -3704,7 +3930,7 @@
       <c r="K49" t="s">
         <v>12</v>
       </c>
-      <c r="L49" s="23"/>
+      <c r="L49" s="24"/>
       <c r="M49" s="18" t="s">
         <v>11</v>
       </c>
@@ -3714,18 +3940,18 @@
       <c r="Q49" t="s">
         <v>12</v>
       </c>
-      <c r="R49" s="23"/>
+      <c r="R49" s="24"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="23"/>
+      <c r="B50" s="24"/>
       <c r="C50" s="13"/>
       <c r="D50" s="13"/>
       <c r="E50" s="13"/>
       <c r="F50" s="13"/>
-      <c r="G50" s="23"/>
+      <c r="G50" s="24"/>
       <c r="I50" t="s">
         <v>13</v>
       </c>
@@ -3735,7 +3961,7 @@
       <c r="K50" t="s">
         <v>11</v>
       </c>
-      <c r="L50" s="23"/>
+      <c r="L50" s="24"/>
       <c r="M50" s="20" t="s">
         <v>21</v>
       </c>
@@ -3745,18 +3971,18 @@
       <c r="Q50" t="s">
         <v>13</v>
       </c>
-      <c r="R50" s="23"/>
+      <c r="R50" s="24"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="23"/>
+      <c r="B51" s="24"/>
       <c r="C51" s="13"/>
       <c r="D51" s="13"/>
       <c r="E51" s="13"/>
       <c r="F51" s="13"/>
-      <c r="G51" s="23"/>
+      <c r="G51" s="24"/>
       <c r="I51" t="s">
         <v>10</v>
       </c>
@@ -3764,7 +3990,7 @@
         <v>12</v>
       </c>
       <c r="K51" s="4"/>
-      <c r="L51" s="23"/>
+      <c r="L51" s="24"/>
       <c r="M51" s="18" t="s">
         <v>21</v>
       </c>
@@ -3774,18 +4000,18 @@
       <c r="Q51" t="s">
         <v>10</v>
       </c>
-      <c r="R51" s="23"/>
+      <c r="R51" s="24"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52" s="23"/>
+      <c r="B52" s="24"/>
       <c r="C52" s="13"/>
       <c r="D52" s="13"/>
       <c r="E52" s="13"/>
       <c r="F52" s="13"/>
-      <c r="G52" s="23"/>
+      <c r="G52" s="24"/>
       <c r="I52" t="s">
         <v>12</v>
       </c>
@@ -3795,7 +4021,7 @@
       <c r="K52" t="s">
         <v>10</v>
       </c>
-      <c r="L52" s="23"/>
+      <c r="L52" s="24"/>
       <c r="M52" s="20" t="s">
         <v>11</v>
       </c>
@@ -3805,18 +4031,18 @@
       <c r="Q52" t="s">
         <v>12</v>
       </c>
-      <c r="R52" s="23"/>
+      <c r="R52" s="24"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" s="23"/>
+      <c r="B53" s="24"/>
       <c r="C53" s="13"/>
       <c r="D53" s="13"/>
       <c r="E53" s="13"/>
       <c r="F53" s="13"/>
-      <c r="G53" s="23"/>
+      <c r="G53" s="24"/>
       <c r="I53" t="s">
         <v>10</v>
       </c>
@@ -3826,22 +4052,22 @@
       <c r="K53" t="s">
         <v>10</v>
       </c>
-      <c r="L53" s="23"/>
+      <c r="L53" s="24"/>
       <c r="Q53" t="s">
         <v>10</v>
       </c>
-      <c r="R53" s="23"/>
+      <c r="R53" s="24"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
-      <c r="B54" s="23"/>
+      <c r="B54" s="24"/>
       <c r="C54" s="13"/>
       <c r="D54" s="13"/>
       <c r="E54" s="13"/>
       <c r="F54" s="13"/>
-      <c r="G54" s="23"/>
+      <c r="G54" s="24"/>
       <c r="I54" t="s">
         <v>21</v>
       </c>
@@ -3851,22 +4077,22 @@
       <c r="K54" t="s">
         <v>13</v>
       </c>
-      <c r="L54" s="23"/>
+      <c r="L54" s="24"/>
       <c r="Q54" t="s">
         <v>171</v>
       </c>
-      <c r="R54" s="23"/>
+      <c r="R54" s="24"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
-      <c r="B55" s="23"/>
+      <c r="B55" s="24"/>
       <c r="C55" s="13"/>
       <c r="D55" s="13"/>
       <c r="E55" s="13"/>
       <c r="F55" s="13"/>
-      <c r="G55" s="23"/>
+      <c r="G55" s="24"/>
       <c r="I55">
         <v>12.5</v>
       </c>
@@ -3876,22 +4102,22 @@
       <c r="K55" t="s">
         <v>13</v>
       </c>
-      <c r="L55" s="23"/>
+      <c r="L55" s="24"/>
       <c r="Q55" t="s">
         <v>13</v>
       </c>
-      <c r="R55" s="23"/>
+      <c r="R55" s="24"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
-      <c r="B56" s="23"/>
+      <c r="B56" s="24"/>
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
-      <c r="G56" s="23"/>
+      <c r="G56" s="24"/>
       <c r="I56" s="3">
         <v>9</v>
       </c>
@@ -3901,246 +4127,246 @@
       <c r="K56" t="s">
         <v>13</v>
       </c>
-      <c r="L56" s="23"/>
+      <c r="L56" s="24"/>
       <c r="Q56" t="s">
         <v>10</v>
       </c>
-      <c r="R56" s="23"/>
+      <c r="R56" s="24"/>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
-      <c r="B57" s="23"/>
+      <c r="B57" s="24"/>
       <c r="F57"/>
-      <c r="G57" s="23"/>
+      <c r="G57" s="24"/>
       <c r="K57" t="s">
         <v>10</v>
       </c>
-      <c r="L57" s="23"/>
+      <c r="L57" s="24"/>
       <c r="Q57" s="4"/>
-      <c r="R57" s="23"/>
+      <c r="R57" s="24"/>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
-      <c r="B58" s="23"/>
+      <c r="B58" s="24"/>
       <c r="F58"/>
-      <c r="G58" s="23"/>
+      <c r="G58" s="24"/>
       <c r="K58" t="s">
         <v>13</v>
       </c>
-      <c r="L58" s="23"/>
-      <c r="R58" s="23"/>
+      <c r="L58" s="24"/>
+      <c r="R58" s="24"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
-      <c r="B59" s="23"/>
+      <c r="B59" s="24"/>
       <c r="F59"/>
-      <c r="G59" s="23"/>
+      <c r="G59" s="24"/>
       <c r="K59" t="s">
         <v>12</v>
       </c>
-      <c r="L59" s="23"/>
-      <c r="R59" s="23"/>
+      <c r="L59" s="24"/>
+      <c r="R59" s="24"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
-      <c r="B60" s="23"/>
+      <c r="B60" s="24"/>
       <c r="F60"/>
-      <c r="G60" s="23"/>
+      <c r="G60" s="24"/>
       <c r="K60">
         <v>0</v>
       </c>
-      <c r="L60" s="23"/>
-      <c r="R60" s="23"/>
+      <c r="L60" s="24"/>
+      <c r="R60" s="24"/>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
-      <c r="B61" s="23"/>
+      <c r="B61" s="24"/>
       <c r="F61"/>
-      <c r="G61" s="23"/>
+      <c r="G61" s="24"/>
       <c r="K61">
         <v>2</v>
       </c>
-      <c r="L61" s="23"/>
-      <c r="R61" s="23"/>
+      <c r="L61" s="24"/>
+      <c r="R61" s="24"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
-      <c r="B62" s="23"/>
+      <c r="B62" s="24"/>
       <c r="F62"/>
-      <c r="G62" s="23"/>
+      <c r="G62" s="24"/>
       <c r="K62" s="3">
         <v>24</v>
       </c>
-      <c r="L62" s="23"/>
-      <c r="R62" s="23"/>
+      <c r="L62" s="24"/>
+      <c r="R62" s="24"/>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
-      <c r="B63" s="23"/>
+      <c r="B63" s="24"/>
       <c r="F63"/>
-      <c r="G63" s="23"/>
+      <c r="G63" s="24"/>
       <c r="K63" t="s">
         <v>13</v>
       </c>
-      <c r="L63" s="23"/>
-      <c r="R63" s="23"/>
+      <c r="L63" s="24"/>
+      <c r="R63" s="24"/>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
-      <c r="B64" s="23"/>
+      <c r="B64" s="24"/>
       <c r="F64"/>
-      <c r="G64" s="23"/>
+      <c r="G64" s="24"/>
       <c r="K64" s="3">
         <v>25</v>
       </c>
-      <c r="L64" s="23"/>
-      <c r="R64" s="23"/>
+      <c r="L64" s="24"/>
+      <c r="R64" s="24"/>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
-      <c r="B65" s="23"/>
+      <c r="B65" s="24"/>
       <c r="F65"/>
-      <c r="G65" s="23"/>
+      <c r="G65" s="24"/>
       <c r="K65">
         <v>317</v>
       </c>
-      <c r="L65" s="23"/>
-      <c r="R65" s="23"/>
+      <c r="L65" s="24"/>
+      <c r="R65" s="24"/>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
-      <c r="B66" s="23"/>
+      <c r="B66" s="24"/>
       <c r="F66"/>
-      <c r="G66" s="23"/>
+      <c r="G66" s="24"/>
       <c r="K66" s="3">
         <v>2</v>
       </c>
-      <c r="L66" s="23"/>
-      <c r="R66" s="23"/>
+      <c r="L66" s="24"/>
+      <c r="R66" s="24"/>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
-      <c r="B67" s="23"/>
+      <c r="B67" s="24"/>
       <c r="F67"/>
-      <c r="G67" s="23"/>
+      <c r="G67" s="24"/>
       <c r="K67">
         <v>11</v>
       </c>
-      <c r="L67" s="23"/>
-      <c r="R67" s="23"/>
+      <c r="L67" s="24"/>
+      <c r="R67" s="24"/>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
-      <c r="B68" s="23"/>
+      <c r="B68" s="24"/>
       <c r="F68"/>
-      <c r="G68" s="23"/>
+      <c r="G68" s="24"/>
       <c r="K68" t="s">
         <v>10</v>
       </c>
-      <c r="L68" s="23"/>
-      <c r="R68" s="23"/>
+      <c r="L68" s="24"/>
+      <c r="R68" s="24"/>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
-      <c r="B69" s="23"/>
+      <c r="B69" s="24"/>
       <c r="F69"/>
-      <c r="G69" s="23"/>
+      <c r="G69" s="24"/>
       <c r="K69" t="s">
         <v>10</v>
       </c>
-      <c r="L69" s="23"/>
-      <c r="R69" s="23"/>
+      <c r="L69" s="24"/>
+      <c r="R69" s="24"/>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
-      <c r="B70" s="23"/>
+      <c r="B70" s="24"/>
       <c r="F70"/>
-      <c r="G70" s="23"/>
+      <c r="G70" s="24"/>
       <c r="K70" t="s">
         <v>10</v>
       </c>
-      <c r="L70" s="23"/>
-      <c r="R70" s="23"/>
+      <c r="L70" s="24"/>
+      <c r="R70" s="24"/>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
-      <c r="B71" s="23"/>
+      <c r="B71" s="24"/>
       <c r="F71"/>
-      <c r="G71" s="23"/>
+      <c r="G71" s="24"/>
       <c r="K71" t="s">
         <v>13</v>
       </c>
-      <c r="L71" s="23"/>
-      <c r="R71" s="23"/>
+      <c r="L71" s="24"/>
+      <c r="R71" s="24"/>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
-      <c r="B72" s="23"/>
+      <c r="B72" s="24"/>
       <c r="F72"/>
-      <c r="G72" s="23"/>
+      <c r="G72" s="24"/>
       <c r="K72" t="s">
         <v>21</v>
       </c>
-      <c r="L72" s="23"/>
-      <c r="R72" s="23"/>
+      <c r="L72" s="24"/>
+      <c r="R72" s="24"/>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
-      <c r="B73" s="23"/>
+      <c r="B73" s="24"/>
       <c r="F73"/>
-      <c r="G73" s="23"/>
+      <c r="G73" s="24"/>
       <c r="K73" t="s">
         <v>12</v>
       </c>
-      <c r="L73" s="23"/>
-      <c r="R73" s="23"/>
+      <c r="L73" s="24"/>
+      <c r="R73" s="24"/>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
-      <c r="B74" s="23"/>
+      <c r="B74" s="24"/>
       <c r="F74"/>
-      <c r="G74" s="23"/>
+      <c r="G74" s="24"/>
       <c r="K74" t="s">
         <v>10</v>
       </c>
-      <c r="L74" s="23"/>
-      <c r="R74" s="23"/>
+      <c r="L74" s="24"/>
+      <c r="R74" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4156,10 +4382,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA24"/>
+  <dimension ref="A1:AG24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA10" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="AC25" sqref="AC25"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="AH12" sqref="AH12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4174,54 +4400,62 @@
     <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="25" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="30" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="23" t="s">
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24" t="s">
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="Z1" s="23" t="s">
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="Z1" s="24" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA1" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="23"/>
+      <c r="B2" s="24"/>
       <c r="C2" s="2"/>
       <c r="E2" s="2">
         <v>44547</v>
@@ -4235,7 +4469,7 @@
       <c r="H2" s="2">
         <v>44548</v>
       </c>
-      <c r="I2" s="23"/>
+      <c r="I2" s="24"/>
       <c r="J2" s="2">
         <v>44553</v>
       </c>
@@ -4284,16 +4518,34 @@
       <c r="Y2" s="2">
         <v>44556</v>
       </c>
-      <c r="Z2" s="23"/>
+      <c r="Z2" s="24"/>
       <c r="AA2" s="2">
         <v>44558</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB2" s="2">
+        <v>44558</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>44560</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>44560</v>
+      </c>
+      <c r="AE2" s="28">
+        <v>44561</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>44562</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>44562</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="7" t="s">
         <v>40</v>
       </c>
@@ -4312,7 +4564,7 @@
       <c r="H3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="23"/>
+      <c r="I3" s="24"/>
       <c r="J3" s="1" t="s">
         <v>151</v>
       </c>
@@ -4361,16 +4613,34 @@
       <c r="Y3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Z3" s="23"/>
+      <c r="Z3" s="24"/>
       <c r="AA3" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="AE3" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="23"/>
+      <c r="B4" s="24"/>
       <c r="C4" t="s">
         <v>11</v>
       </c>
@@ -4389,7 +4659,7 @@
       <c r="H4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="23"/>
+      <c r="I4" s="24"/>
       <c r="J4">
         <v>256</v>
       </c>
@@ -4436,16 +4706,34 @@
       <c r="Y4" t="s">
         <v>10</v>
       </c>
-      <c r="Z4" s="23"/>
+      <c r="Z4" s="24"/>
       <c r="AA4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="AC4">
+        <v>32</v>
+      </c>
+      <c r="AD4" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="AE4" s="5">
+        <v>100</v>
+      </c>
+      <c r="AF4">
+        <v>17</v>
+      </c>
+      <c r="AG4" s="3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="23"/>
+      <c r="B5" s="24"/>
       <c r="C5" t="s">
         <v>12</v>
       </c>
@@ -4464,7 +4752,7 @@
       <c r="H5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="23"/>
+      <c r="I5" s="24"/>
       <c r="J5">
         <v>13</v>
       </c>
@@ -4509,16 +4797,34 @@
       <c r="Y5" t="s">
         <v>21</v>
       </c>
-      <c r="Z5" s="23"/>
-      <c r="AA5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z5" s="24"/>
+      <c r="AA5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>25</v>
+      </c>
+      <c r="AD5" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="AE5" s="5">
+        <v>45</v>
+      </c>
+      <c r="AF5">
+        <v>10.4</v>
+      </c>
+      <c r="AG5" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="23"/>
+      <c r="B6" s="24"/>
       <c r="C6" t="s">
         <v>13</v>
       </c>
@@ -4537,7 +4843,7 @@
       <c r="H6" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="23"/>
+      <c r="I6" s="24"/>
       <c r="J6" s="3">
         <v>38</v>
       </c>
@@ -4584,16 +4890,32 @@
       <c r="Y6" t="s">
         <v>10</v>
       </c>
-      <c r="Z6" s="23"/>
+      <c r="Z6" s="24"/>
       <c r="AA6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB6" t="s">
+        <v>229</v>
+      </c>
+      <c r="AC6">
+        <v>45</v>
+      </c>
+      <c r="AD6" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="AE6" s="5">
+        <v>11</v>
+      </c>
+      <c r="AF6">
+        <v>2</v>
+      </c>
+      <c r="AG6" s="4"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="24"/>
       <c r="C7">
         <v>-15</v>
       </c>
@@ -4610,7 +4932,7 @@
         <v>75</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="23"/>
+      <c r="I7" s="24"/>
       <c r="J7" s="3">
         <v>400</v>
       </c>
@@ -4654,16 +4976,32 @@
       <c r="Y7" t="s">
         <v>10</v>
       </c>
-      <c r="Z7" s="23"/>
+      <c r="Z7" s="24"/>
       <c r="AA7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB7" s="4"/>
+      <c r="AC7">
+        <v>40</v>
+      </c>
+      <c r="AD7" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="AE7" s="5">
+        <v>43</v>
+      </c>
+      <c r="AF7">
+        <v>20</v>
+      </c>
+      <c r="AG7" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="23"/>
+      <c r="B8" s="24"/>
       <c r="C8" t="s">
         <v>11</v>
       </c>
@@ -4682,7 +5020,7 @@
       <c r="H8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="23"/>
+      <c r="I8" s="24"/>
       <c r="J8" t="s">
         <v>146</v>
       </c>
@@ -4726,16 +5064,34 @@
       <c r="Y8">
         <v>17</v>
       </c>
-      <c r="Z8" s="23"/>
-      <c r="AA8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z8" s="24"/>
+      <c r="AA8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>50</v>
+      </c>
+      <c r="AC8">
+        <v>52</v>
+      </c>
+      <c r="AD8" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="AE8" s="5">
+        <v>108</v>
+      </c>
+      <c r="AF8" s="5">
+        <v>8</v>
+      </c>
+      <c r="AG8" s="3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" s="23"/>
+      <c r="B9" s="24"/>
       <c r="C9" t="s">
         <v>12</v>
       </c>
@@ -4754,7 +5110,7 @@
       <c r="H9">
         <v>25</v>
       </c>
-      <c r="I9" s="23"/>
+      <c r="I9" s="24"/>
       <c r="J9" s="4"/>
       <c r="K9" s="3">
         <v>80</v>
@@ -4795,16 +5151,34 @@
       <c r="Y9" t="s">
         <v>13</v>
       </c>
-      <c r="Z9" s="23"/>
+      <c r="Z9" s="24"/>
       <c r="AA9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB9" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>11</v>
+      </c>
+      <c r="AD9" s="5">
+        <v>12</v>
+      </c>
+      <c r="AE9" s="5">
+        <v>33</v>
+      </c>
+      <c r="AF9" s="5">
+        <v>360</v>
+      </c>
+      <c r="AG9" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" s="23"/>
+      <c r="B10" s="24"/>
       <c r="C10" t="s">
         <v>10</v>
       </c>
@@ -4823,7 +5197,7 @@
       <c r="H10" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="23"/>
+      <c r="I10" s="24"/>
       <c r="J10" s="3" t="s">
         <v>147</v>
       </c>
@@ -4866,16 +5240,34 @@
       <c r="Y10" t="s">
         <v>21</v>
       </c>
-      <c r="Z10" s="23"/>
+      <c r="Z10" s="24"/>
       <c r="AA10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB10" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="AC10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD10" s="5">
+        <v>3</v>
+      </c>
+      <c r="AE10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF10" s="3">
+        <v>31</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11" s="23"/>
+      <c r="B11" s="24"/>
       <c r="C11" t="s">
         <v>10</v>
       </c>
@@ -4892,7 +5284,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="4"/>
-      <c r="I11" s="23"/>
+      <c r="I11" s="24"/>
       <c r="J11" t="s">
         <v>148</v>
       </c>
@@ -4930,16 +5322,32 @@
       <c r="Y11" t="s">
         <v>12</v>
       </c>
-      <c r="Z11" s="23"/>
+      <c r="Z11" s="24"/>
       <c r="AA11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="AB11" s="4"/>
+      <c r="AC11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF11" s="5">
+        <v>5</v>
+      </c>
+      <c r="AG11" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
-      <c r="B12" s="23"/>
+      <c r="B12" s="24"/>
       <c r="C12">
         <v>-1</v>
       </c>
@@ -4958,7 +5366,7 @@
       <c r="H12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="23"/>
+      <c r="I12" s="24"/>
       <c r="J12" t="s">
         <v>149</v>
       </c>
@@ -4998,16 +5406,34 @@
       <c r="Y12" t="s">
         <v>13</v>
       </c>
-      <c r="Z12" s="23"/>
+      <c r="Z12" s="24"/>
       <c r="AA12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB12" s="3">
+        <v>204</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD12" s="5">
+        <v>74.48</v>
+      </c>
+      <c r="AE12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF12" s="3">
+        <v>3510</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
-      <c r="B13" s="23"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
@@ -5023,7 +5449,7 @@
       <c r="H13" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="23"/>
+      <c r="I13" s="24"/>
       <c r="J13" t="s">
         <v>150</v>
       </c>
@@ -5061,16 +5487,25 @@
       <c r="Y13" t="s">
         <v>11</v>
       </c>
-      <c r="Z13" s="23"/>
+      <c r="Z13" s="24"/>
       <c r="AA13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB13" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD13" s="5">
+        <v>44.44</v>
+      </c>
+      <c r="AF13" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
-      <c r="B14" s="23"/>
+      <c r="B14" s="24"/>
       <c r="C14" t="s">
         <v>13</v>
       </c>
@@ -5087,7 +5522,7 @@
         <v>60</v>
       </c>
       <c r="H14" s="4"/>
-      <c r="I14" s="23"/>
+      <c r="I14" s="24"/>
       <c r="J14" s="4"/>
       <c r="K14" s="15" t="s">
         <v>154</v>
@@ -5121,16 +5556,21 @@
       <c r="Y14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Z14" s="23"/>
+      <c r="Z14" s="24"/>
       <c r="AA14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB14" s="3">
+        <v>196</v>
+      </c>
+      <c r="AD14" s="4"/>
+      <c r="AF14" s="4"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
-      <c r="B15" s="23"/>
+      <c r="B15" s="24"/>
       <c r="C15" t="s">
         <v>21</v>
       </c>
@@ -5149,7 +5589,7 @@
       <c r="H15" s="3">
         <v>27</v>
       </c>
-      <c r="I15" s="23"/>
+      <c r="I15" s="24"/>
       <c r="J15" s="3" t="s">
         <v>12</v>
       </c>
@@ -5182,16 +5622,25 @@
       <c r="Y15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="Z15" s="23"/>
+      <c r="Z15" s="24"/>
       <c r="AA15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB15" t="s">
+        <v>228</v>
+      </c>
+      <c r="AD15" s="5">
+        <v>5</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
-      <c r="B16" s="23"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="3">
         <v>600</v>
       </c>
@@ -5206,7 +5655,7 @@
         <v>10</v>
       </c>
       <c r="H16" s="4"/>
-      <c r="I16" s="23"/>
+      <c r="I16" s="24"/>
       <c r="J16" t="s">
         <v>13</v>
       </c>
@@ -5239,16 +5688,25 @@
       <c r="Y16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Z16" s="23"/>
+      <c r="Z16" s="24"/>
       <c r="AA16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB16" t="s">
+        <v>228</v>
+      </c>
+      <c r="AD16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF16" s="19" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
-      <c r="B17" s="23"/>
+      <c r="B17" s="24"/>
       <c r="C17" t="s">
         <v>10</v>
       </c>
@@ -5263,7 +5721,7 @@
         <v>10</v>
       </c>
       <c r="H17" s="4"/>
-      <c r="I17" s="23"/>
+      <c r="I17" s="24"/>
       <c r="J17" s="3" t="s">
         <v>13</v>
       </c>
@@ -5298,16 +5756,25 @@
       <c r="Y17" t="s">
         <v>10</v>
       </c>
-      <c r="Z17" s="23"/>
+      <c r="Z17" s="24"/>
       <c r="AA17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB17" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="AD17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF17" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
-      <c r="B18" s="23"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="4"/>
       <c r="D18" t="s">
         <v>13</v>
@@ -5322,7 +5789,7 @@
       <c r="H18" s="3">
         <v>2525</v>
       </c>
-      <c r="I18" s="23"/>
+      <c r="I18" s="24"/>
       <c r="K18">
         <v>160</v>
       </c>
@@ -5351,16 +5818,25 @@
       <c r="Y18" t="s">
         <v>10</v>
       </c>
-      <c r="Z18" s="23"/>
+      <c r="Z18" s="24"/>
       <c r="AA18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB18" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="AD18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF18" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="24"/>
       <c r="C19" t="s">
         <v>13</v>
       </c>
@@ -5379,7 +5855,7 @@
       <c r="H19" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="23"/>
+      <c r="I19" s="24"/>
       <c r="K19">
         <v>20</v>
       </c>
@@ -5401,16 +5877,23 @@
       <c r="Y19" t="s">
         <v>13</v>
       </c>
-      <c r="Z19" s="23"/>
+      <c r="Z19" s="24"/>
       <c r="AA19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB19" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="AD19" s="5"/>
+      <c r="AF19" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
-      <c r="B20" s="23"/>
+      <c r="B20" s="24"/>
       <c r="C20" t="s">
         <v>12</v>
       </c>
@@ -5427,7 +5910,7 @@
       <c r="H20" t="s">
         <v>21</v>
       </c>
-      <c r="I20" s="23"/>
+      <c r="I20" s="24"/>
       <c r="K20">
         <v>28</v>
       </c>
@@ -5447,13 +5930,20 @@
       <c r="Y20" t="s">
         <v>216</v>
       </c>
-      <c r="Z20" s="23"/>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z20" s="24"/>
+      <c r="AA20" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>8</v>
+      </c>
+      <c r="AD20" s="5"/>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
-      <c r="B21" s="23"/>
+      <c r="B21" s="24"/>
       <c r="C21" t="s">
         <v>10</v>
       </c>
@@ -5470,7 +5960,7 @@
       <c r="H21" t="s">
         <v>63</v>
       </c>
-      <c r="I21" s="23"/>
+      <c r="I21" s="24"/>
       <c r="K21">
         <v>200</v>
       </c>
@@ -5492,13 +5982,20 @@
       <c r="Y21">
         <v>15</v>
       </c>
-      <c r="Z21" s="23"/>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z21" s="24"/>
+      <c r="AA21" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB21" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="AD21" s="5"/>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
-      <c r="B22" s="23"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="3" t="s">
         <v>13</v>
       </c>
@@ -5517,7 +6014,7 @@
       <c r="H22" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I22" s="23"/>
+      <c r="I22" s="24"/>
       <c r="K22" t="s">
         <v>12</v>
       </c>
@@ -5530,13 +6027,18 @@
       <c r="Y22" t="s">
         <v>10</v>
       </c>
-      <c r="Z22" s="23"/>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z22" s="24"/>
+      <c r="AA22" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB22" s="4"/>
+      <c r="AD22" s="5"/>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
-      <c r="B23" s="23"/>
+      <c r="B23" s="24"/>
       <c r="C23">
         <v>-70</v>
       </c>
@@ -5555,7 +6057,7 @@
       <c r="H23" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="I23" s="23"/>
+      <c r="I23" s="24"/>
       <c r="K23" t="s">
         <v>10</v>
       </c>
@@ -5568,22 +6070,29 @@
       <c r="Y23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Z23" s="23"/>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z23" s="24"/>
+      <c r="AA23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD23" s="5"/>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="K24" s="3" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B1:B23"/>
+    <mergeCell ref="J1:Q1"/>
     <mergeCell ref="Z1:Z23"/>
     <mergeCell ref="R1:U1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:I23"/>
-    <mergeCell ref="B1:B23"/>
-    <mergeCell ref="J1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5605,7 +6114,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>121</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -5619,7 +6128,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
+      <c r="A2" s="24"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -5628,7 +6137,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="1" t="s">
         <v>41</v>
       </c>
@@ -5640,7 +6149,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="B4" t="s">
         <v>70</v>
       </c>
@@ -5649,7 +6158,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="8" t="s">
         <v>89</v>
       </c>
@@ -5658,7 +6167,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="8" t="s">
         <v>90</v>
       </c>
@@ -5667,7 +6176,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="8" t="s">
         <v>91</v>
       </c>
@@ -5676,7 +6185,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="8" t="s">
         <v>92</v>
       </c>
@@ -5685,7 +6194,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="8" t="s">
         <v>93</v>
       </c>
@@ -5694,7 +6203,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="8" t="s">
         <v>94</v>
       </c>
@@ -5703,7 +6212,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="8" t="s">
         <v>95</v>
       </c>
@@ -5712,7 +6221,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
+      <c r="A12" s="24"/>
       <c r="B12" t="s">
         <v>72</v>
       </c>
@@ -5721,7 +6230,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="B13" t="s">
         <v>96</v>
       </c>
@@ -5731,7 +6240,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" t="s">
         <v>97</v>
       </c>
@@ -5740,7 +6249,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
+      <c r="A15" s="24"/>
       <c r="B15" t="s">
         <v>98</v>
       </c>
@@ -5750,7 +6259,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
+      <c r="A16" s="24"/>
       <c r="B16">
         <v>3</v>
       </c>
@@ -5759,7 +6268,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
+      <c r="A17" s="24"/>
       <c r="B17" t="s">
         <v>75</v>
       </c>
@@ -5768,7 +6277,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
+      <c r="A18" s="24"/>
       <c r="B18" t="s">
         <v>99</v>
       </c>
@@ -5777,7 +6286,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
+      <c r="A19" s="24"/>
       <c r="B19" t="s">
         <v>78</v>
       </c>
@@ -5786,7 +6295,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
+      <c r="A20" s="24"/>
       <c r="B20" t="s">
         <v>100</v>
       </c>
@@ -5795,7 +6304,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
+      <c r="A21" s="24"/>
       <c r="B21">
         <v>6</v>
       </c>
@@ -5804,7 +6313,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
+      <c r="A22" s="24"/>
       <c r="B22">
         <v>7</v>
       </c>
@@ -5813,7 +6322,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
+      <c r="A23" s="24"/>
       <c r="B23" t="s">
         <v>83</v>
       </c>
@@ -5822,7 +6331,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="8" t="s">
         <v>101</v>
       </c>
@@ -5831,7 +6340,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
+      <c r="A25" s="24"/>
       <c r="B25" s="8" t="s">
         <v>102</v>
       </c>
@@ -5840,7 +6349,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
+      <c r="A26" s="24"/>
       <c r="B26" s="8" t="s">
         <v>103</v>
       </c>
@@ -5849,7 +6358,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
+      <c r="A27" s="24"/>
       <c r="B27" s="8" t="s">
         <v>104</v>
       </c>
@@ -5858,7 +6367,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="8" t="s">
         <v>105</v>
       </c>
@@ -5867,7 +6376,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
+      <c r="A29" s="24"/>
       <c r="B29" s="8" t="s">
         <v>106</v>
       </c>
@@ -5876,7 +6385,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
+      <c r="A30" s="24"/>
       <c r="B30" s="8" t="s">
         <v>107</v>
       </c>
@@ -5885,7 +6394,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
+      <c r="A31" s="24"/>
       <c r="B31" s="8" t="s">
         <v>108</v>
       </c>
@@ -5894,7 +6403,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
+      <c r="A32" s="24"/>
       <c r="B32" s="8" t="s">
         <v>109</v>
       </c>
@@ -5903,7 +6412,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
+      <c r="A33" s="24"/>
       <c r="B33" s="8" t="s">
         <v>110</v>
       </c>
@@ -5912,7 +6421,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
+      <c r="A34" s="24"/>
       <c r="B34" s="8" t="s">
         <v>111</v>
       </c>
@@ -5921,7 +6430,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
+      <c r="A35" s="24"/>
       <c r="B35" t="s">
         <v>86</v>
       </c>
@@ -5930,7 +6439,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
+      <c r="A36" s="24"/>
       <c r="B36" t="s">
         <v>112</v>
       </c>
@@ -5939,7 +6448,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
+      <c r="A37" s="24"/>
       <c r="B37" t="s">
         <v>113</v>
       </c>
@@ -5948,7 +6457,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
+      <c r="A38" s="24"/>
       <c r="B38" t="s">
         <v>114</v>
       </c>
@@ -5957,7 +6466,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
+      <c r="A39" s="24"/>
       <c r="B39" t="s">
         <v>114</v>
       </c>
@@ -5966,7 +6475,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
+      <c r="A40" s="24"/>
       <c r="B40">
         <v>10</v>
       </c>
@@ -5975,7 +6484,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
+      <c r="A41" s="24"/>
       <c r="B41">
         <v>11</v>
       </c>
@@ -5984,7 +6493,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
+      <c r="A42" s="24"/>
       <c r="B42">
         <v>12</v>
       </c>
@@ -5993,7 +6502,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
+      <c r="A43" s="24"/>
       <c r="B43">
         <v>13</v>
       </c>
@@ -6002,7 +6511,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
+      <c r="A44" s="24"/>
       <c r="B44" t="s">
         <v>115</v>
       </c>
@@ -6011,7 +6520,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
+      <c r="A45" s="24"/>
       <c r="B45" t="s">
         <v>116</v>
       </c>
@@ -6020,7 +6529,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
+      <c r="A46" s="24"/>
       <c r="B46" t="s">
         <v>117</v>
       </c>
@@ -6029,7 +6538,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
+      <c r="A47" s="24"/>
       <c r="B47" t="s">
         <v>118</v>
       </c>
@@ -6038,7 +6547,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
+      <c r="A48" s="24"/>
       <c r="B48" t="s">
         <v>119</v>
       </c>
@@ -6047,7 +6556,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
+      <c r="A49" s="24"/>
       <c r="B49" t="s">
         <v>120</v>
       </c>
@@ -6056,7 +6565,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
+      <c r="A50" s="24"/>
       <c r="B50">
         <v>15</v>
       </c>

</xml_diff>